<commit_message>
Implement new capacity payment calculation method based on electricity system needs, brief calibration of CRtPaL-profits, enable cost-driven retirements (#232)
</commit_message>
<xml_diff>
--- a/InputData/elec/CRtPaL/Capacity Responses to Profits and Losses.xlsx
+++ b/InputData/elec/CRtPaL/Capacity Responses to Profits and Losses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\CRtPaL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D964641-3A0A-4B75-B57C-D3DE9B21D9FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC331801-3C56-4B0C-B171-5BA51EB8B568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29220" yWindow="4515" windowWidth="20010" windowHeight="18315" xr2:uid="{7BF3F63E-6BCA-416F-BEB8-BA0404DF6A3E}"/>
+    <workbookView xWindow="1515" yWindow="7545" windowWidth="11475" windowHeight="13995" xr2:uid="{7BF3F63E-6BCA-416F-BEB8-BA0404DF6A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>CRtPaL Capacity Response to Profits</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>change in capacity</t>
+  </si>
+  <si>
+    <t>Calibrated</t>
   </si>
 </sst>
 </file>
@@ -502,7 +505,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9CF6A6C-E998-448A-8CB8-3A5997ADF63A}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -511,42 +514,45 @@
     <col min="1" max="1" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -604,7 +610,7 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +618,7 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,7 +626,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +634,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +642,7 @@
         <v>17</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +650,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -652,7 +658,7 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +666,7 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,7 +674,7 @@
         <v>21</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -676,7 +682,7 @@
         <v>22</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -684,7 +690,7 @@
         <v>23</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -692,7 +698,7 @@
         <v>24</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -700,7 +706,7 @@
         <v>25</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -708,7 +714,7 @@
         <v>26</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -716,7 +722,7 @@
         <v>27</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -724,7 +730,7 @@
         <v>28</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -732,7 +738,7 @@
         <v>29</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calibrate capacity addition and retirement parameters
</commit_message>
<xml_diff>
--- a/InputData/elec/CRtPaL/Capacity Responses to Profits and Losses.xlsx
+++ b/InputData/elec/CRtPaL/Capacity Responses to Profits and Losses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\CRtPaL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\CRtPaL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC331801-3C56-4B0C-B171-5BA51EB8B568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC93CB9D-3B03-426D-9B69-8BDC7B8F2AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="7545" windowWidth="11475" windowHeight="13995" xr2:uid="{7BF3F63E-6BCA-416F-BEB8-BA0404DF6A3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{7BF3F63E-6BCA-416F-BEB8-BA0404DF6A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -589,7 +589,9 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -610,7 +612,7 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -618,7 +620,7 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -626,7 +628,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -634,7 +636,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>0.02</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,7 +644,7 @@
         <v>17</v>
       </c>
       <c r="B6">
-        <v>0.02</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -650,7 +652,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>0.7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -658,7 +660,7 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>0.75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -666,7 +668,7 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -674,7 +676,7 @@
         <v>21</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -682,7 +684,7 @@
         <v>22</v>
       </c>
       <c r="B11">
-        <v>0.02</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -690,7 +692,7 @@
         <v>23</v>
       </c>
       <c r="B12">
-        <v>0.02</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -698,7 +700,7 @@
         <v>24</v>
       </c>
       <c r="B13">
-        <v>0.15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -706,7 +708,7 @@
         <v>25</v>
       </c>
       <c r="B14">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -714,7 +716,7 @@
         <v>26</v>
       </c>
       <c r="B15">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Data and structural updates based on calibration.
</commit_message>
<xml_diff>
--- a/InputData/elec/CRtPaL/Capacity Responses to Profits and Losses.xlsx
+++ b/InputData/elec/CRtPaL/Capacity Responses to Profits and Losses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CRtPaL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE167A3E-C33B-4000-B63A-BDAC275D265A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D78E4BC-2FE0-4592-88DD-F698C9537CE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="1" xr2:uid="{7BF3F63E-6BCA-416F-BEB8-BA0404DF6A3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{7BF3F63E-6BCA-416F-BEB8-BA0404DF6A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9CF6A6C-E998-448A-8CB8-3A5997ADF63A}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -608,8 +608,8 @@
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -647,7 +647,7 @@
         <v>15</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -655,7 +655,7 @@
         <v>16</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
         <v>17</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -671,7 +671,7 @@
         <v>18</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -679,7 +679,7 @@
         <v>19</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -687,7 +687,7 @@
         <v>20</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -695,7 +695,7 @@
         <v>21</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
         <v>22</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -711,7 +711,7 @@
         <v>23</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -719,7 +719,7 @@
         <v>24</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
         <v>25</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -735,7 +735,7 @@
         <v>26</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -743,7 +743,7 @@
         <v>27</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
         <v>28</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -759,7 +759,7 @@
         <v>29</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>32</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -775,7 +775,7 @@
         <v>33</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -783,7 +783,7 @@
         <v>34</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -791,7 +791,7 @@
         <v>35</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
         <v>36</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
         <v>37</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>